<commit_message>
[Closed] escape first n rows, sheet name or number #1 https://github.com/basakpie/vaadin-exceluploader-addon/issues/1
</commit_message>
<xml_diff>
--- a/exceluploader-addon/src/test/resources/annotation_upload.xlsx
+++ b/exceluploader-addon/src/test/resources/annotation_upload.xlsx
@@ -5,21 +5,22 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\basakpie\vaadin-exceluploader-addon\exceluploader-addon\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\git\vaadin-exceluploader-addon\exceluploader-addon\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13695"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13695" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>아이디</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -37,59 +38,107 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>1_xlsx@email.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2_xlsx@email.com</t>
+  </si>
+  <si>
+    <t>3_xlsx@email.com</t>
+  </si>
+  <si>
+    <t>4_xlsx@email.com</t>
+  </si>
+  <si>
+    <t>5_xlsx@email.com</t>
+  </si>
+  <si>
+    <t>title</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>subtitle1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>subtitle2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1_option_name_xlsx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2_option_name_xlsx</t>
+  </si>
+  <si>
+    <t>3_option_name_xlsx</t>
+  </si>
+  <si>
+    <t>5_option_name_xlsx</t>
+  </si>
+  <si>
+    <t>6_option_name_xlsx</t>
+  </si>
+  <si>
+    <t>7_option_name_xlsx</t>
+  </si>
+  <si>
+    <t>8_option_name_xlsx</t>
+  </si>
+  <si>
+    <t>1_option_xlsx@email.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2_option_xlsx@email.com</t>
+  </si>
+  <si>
+    <t>3_option_xlsx@email.com</t>
+  </si>
+  <si>
+    <t>4_option_xlsx@email.com</t>
+  </si>
+  <si>
+    <t>5_option_xlsx@email.com</t>
+  </si>
+  <si>
+    <t>7_option_xlsx@email.com</t>
+  </si>
+  <si>
+    <t>8_option_xlsx@email.com</t>
+  </si>
+  <si>
     <t>2_name_xlsx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>3_name_xlsx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>5_name_xlsx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>6_name_xlsx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>7_name_xlsx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>8_name_xlsx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1_xlsx@email.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2_xlsx@email.com</t>
-  </si>
-  <si>
-    <t>3_xlsx@email.com</t>
-  </si>
-  <si>
-    <t>4_xlsx@email.com</t>
-  </si>
-  <si>
-    <t>5_xlsx@email.com</t>
   </si>
   <si>
     <t>7_xlsx@email.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>8_xlsx@email.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +152,13 @@
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -127,9 +183,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -413,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -442,7 +504,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -450,10 +512,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -461,10 +523,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -472,7 +534,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -480,10 +542,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -491,7 +553,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -499,10 +561,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -510,10 +572,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -521,4 +583,138 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.625" customWidth="1"/>
+    <col min="3" max="3" width="14.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:B2"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>